<commit_message>
add some more assets?
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="82">
   <si>
     <t>Asset</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Smartshares NZ Top 50</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -281,12 +278,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -310,6 +301,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -340,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -348,25 +345,22 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -375,26 +369,23 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,12 +695,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="18" width="57.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="57.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -720,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -731,7 +722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
@@ -742,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
@@ -753,7 +744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="12" t="s">
         <v>25</v>
       </c>
@@ -764,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
@@ -775,7 +766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="12" t="s">
         <v>33</v>
       </c>
@@ -786,7 +777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="12" t="s">
         <v>37</v>
       </c>
@@ -797,290 +788,290 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>82</v>
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>82</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>82</v>
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>82</v>
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>82</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>82</v>
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>82</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>82</v>
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>82</v>
+        <v>46</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>82</v>
+        <v>51</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>82</v>
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>82</v>
+        <v>56</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>82</v>
+        <v>60</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>82</v>
+        <v>62</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>82</v>
+        <v>64</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>82</v>
+        <v>66</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="56.25">
       <c r="A30" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>82</v>
+        <v>72</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="37.5">
       <c r="A31" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1099,17 +1090,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1128,10 +1119,10 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -1161,7 +1152,7 @@
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1186,7 +1177,7 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1211,7 +1202,7 @@
       <c r="E4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1236,7 +1227,7 @@
       <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1261,7 +1252,7 @@
       <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1286,7 +1277,7 @@
       <c r="E7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1311,7 +1302,7 @@
       <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1336,7 +1327,7 @@
       <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1361,7 +1352,7 @@
       <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -1386,7 +1377,7 @@
       <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -1411,7 +1402,7 @@
       <c r="E12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -1436,7 +1427,7 @@
       <c r="E13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>52</v>
       </c>
       <c r="G13" s="4" t="s">
@@ -1461,7 +1452,7 @@
       <c r="E14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>54</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1486,7 +1477,7 @@
       <c r="E15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>57</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -1511,7 +1502,7 @@
       <c r="E16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>59</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -1536,7 +1527,7 @@
       <c r="E17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G17" s="4" t="s">
@@ -1561,7 +1552,7 @@
       <c r="E18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>63</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1586,7 +1577,7 @@
       <c r="E19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -1611,7 +1602,7 @@
       <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -1636,7 +1627,7 @@
       <c r="E21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>69</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1661,7 +1652,7 @@
       <c r="E22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>71</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -1736,7 +1727,7 @@
       <c r="E25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3" t="s">
         <v>77</v>
       </c>
       <c r="G25" s="4" t="s">
@@ -1761,7 +1752,7 @@
       <c r="E26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -1786,7 +1777,7 @@
       <c r="E27" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>81</v>
       </c>
       <c r="G27" s="4" t="s">
@@ -1809,8 +1800,8 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="1"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1828,8 +1819,8 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="1"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1839,7 +1830,7 @@
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1847,8 +1838,8 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="1"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1858,7 +1849,7 @@
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1866,8 +1857,8 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="1"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1885,8 +1876,8 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="1"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1904,8 +1895,8 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1923,164 +1914,164 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="1"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="1"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="1"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="1"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="1"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="1"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="1"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B41" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="1"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="1"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3"/>
+      <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2091,21 +2082,21 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="1"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3"/>
+      <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="1"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2123,8 +2114,8 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="1"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2142,8 +2133,8 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="1"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2161,8 +2152,8 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="9"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="8"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2180,8 +2171,8 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="9"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="8"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>

</xml_diff>

<commit_message>
adding some more assets, this looks good
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="82">
   <si>
     <t>Asset</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>Smartshares NZ Top 50</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -340,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -348,11 +345,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -378,16 +372,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -701,383 +692,383 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="57.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="57.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>82</v>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>82</v>
+      <c r="A24" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>82</v>
+      <c r="A25" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>82</v>
+      <c r="A26" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>82</v>
+      <c r="A27" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>82</v>
+      <c r="A28" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>82</v>
+      <c r="A29" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="56.25">
-      <c r="A30" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>82</v>
+      <c r="A30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="37.5">
-      <c r="A31" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>82</v>
+      <c r="A31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>82</v>
+      <c r="A32" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>82</v>
+      <c r="A33" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>82</v>
+      <c r="A34" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1096,17 +1087,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1161,7 +1152,7 @@
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2"/>
@@ -1186,7 +1177,7 @@
       <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="2"/>
@@ -1211,7 +1202,7 @@
       <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="2"/>
@@ -1236,7 +1227,7 @@
       <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="2"/>
@@ -1261,7 +1252,7 @@
       <c r="F6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="2"/>
@@ -1286,7 +1277,7 @@
       <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="2"/>
@@ -1311,7 +1302,7 @@
       <c r="F8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="2"/>
@@ -1336,7 +1327,7 @@
       <c r="F9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H9" s="2"/>
@@ -1361,7 +1352,7 @@
       <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="2"/>
@@ -1386,7 +1377,7 @@
       <c r="F11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H11" s="2"/>
@@ -1411,7 +1402,7 @@
       <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H12" s="2"/>
@@ -1436,7 +1427,7 @@
       <c r="F13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="1" t="s">
         <v>50</v>
       </c>
       <c r="H13" s="2"/>
@@ -1461,7 +1452,7 @@
       <c r="F14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="2"/>
@@ -1486,7 +1477,7 @@
       <c r="F15" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H15" s="2"/>
@@ -1511,7 +1502,7 @@
       <c r="F16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H16" s="2"/>
@@ -1536,7 +1527,7 @@
       <c r="F17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H17" s="2"/>
@@ -1561,7 +1552,7 @@
       <c r="F18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H18" s="2"/>
@@ -1586,7 +1577,7 @@
       <c r="F19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H19" s="2"/>
@@ -1611,7 +1602,7 @@
       <c r="F20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H20" s="2"/>
@@ -1636,7 +1627,7 @@
       <c r="F21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H21" s="2"/>
@@ -1661,7 +1652,7 @@
       <c r="F22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H22" s="2"/>
@@ -1683,10 +1674,10 @@
       <c r="E23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="2"/>
@@ -1708,10 +1699,10 @@
       <c r="E24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H24" s="2"/>
@@ -1736,7 +1727,7 @@
       <c r="F25" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H25" s="2"/>
@@ -1761,7 +1752,7 @@
       <c r="F26" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H26" s="2"/>
@@ -1786,7 +1777,7 @@
       <c r="F27" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="G27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="H27" s="2"/>
@@ -1836,7 +1827,7 @@
       <c r="A30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1855,7 +1846,7 @@
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1928,10 +1919,10 @@
       <c r="K34" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="2"/>
@@ -1945,10 +1936,10 @@
       <c r="K35" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="2"/>
@@ -1962,10 +1953,10 @@
       <c r="K36" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="2"/>
@@ -1979,10 +1970,10 @@
       <c r="K37" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="2"/>
@@ -1996,10 +1987,10 @@
       <c r="K38" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C39" s="2"/>
@@ -2013,10 +2004,10 @@
       <c r="K39" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="2"/>
@@ -2030,10 +2021,10 @@
       <c r="K40" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C41" s="2"/>
@@ -2047,10 +2038,10 @@
       <c r="K41" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="2"/>
@@ -2109,7 +2100,7 @@
       <c r="K45" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2128,7 +2119,7 @@
       <c r="K46" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="4" t="s">
+      <c r="A47" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2147,7 +2138,7 @@
       <c r="K47" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="4" t="s">
+      <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -2159,14 +2150,14 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="8"/>
+      <c r="G48" s="7"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2178,7 +2169,7 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="3"/>
-      <c r="G49" s="8"/>
+      <c r="G49" s="7"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>

</xml_diff>

<commit_message>
lets see how we go
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="84">
   <si>
     <t>Asset</t>
   </si>
@@ -326,13 +326,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -355,11 +355,8 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -666,210 +663,210 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="57.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="57.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>28</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>41</v>
+        <v>63</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>62</v>
+        <v>81</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>82</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>17</v>
+        <v>65</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>66</v>
+        <v>37</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <v>39</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>38</v>
+        <v>67</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>83</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>56</v>
@@ -877,54 +874,54 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="10" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>15</v>
+        <v>59</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>15</v>
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>60</v>
+        <v>71</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>56</v>
@@ -932,10 +929,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>13</v>
@@ -943,10 +940,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>32</v>
+        <v>79</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>20</v>
@@ -954,65 +951,65 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>72</v>
+        <v>79</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>34</v>
+        <v>23</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="21">
       <c r="A29" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>80</v>
+        <v>75</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>80</v>
+        <v>54</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>24</v>
+        <v>77</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>20</v>
@@ -1020,110 +1017,66 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="10" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>55</v>
+        <v>69</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>20</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="56.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="37.5">
+      <c r="A36" s="10"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="56.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+      <c r="A38" s="10"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="10"/>
       <c r="B39" s="4"/>
       <c r="C39" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="37.5">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="10"/>
       <c r="B40" s="4"/>
       <c r="C40" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="10"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="10"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
making some more work!
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="90">
   <si>
     <t>Asset</t>
   </si>
@@ -286,9 +286,6 @@
   <si>
     <t xml:space="preserve">iShares US Healthcare ETF
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bonds </t>
   </si>
   <si>
     <t>Housing</t>
@@ -922,7 +919,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -955,7 +952,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
is this gonna work
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="92">
   <si>
     <t>Asset</t>
   </si>
@@ -281,6 +281,9 @@
     <t>Metals</t>
   </si>
   <si>
+    <t>ITA</t>
+  </si>
+  <si>
     <t>Defense</t>
   </si>
   <si>
@@ -288,10 +291,10 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Bonds </t>
+  </si>
+  <si>
     <t>Housing</t>
-  </si>
-  <si>
-    <t>Bond</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -762,87 +765,87 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="8" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>19</v>
+        <v>82</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="8" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="8" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="8" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="8" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>56</v>
@@ -850,10 +853,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="8" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>56</v>
@@ -861,21 +864,21 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="8" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>83</v>
@@ -883,147 +886,153 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="8" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="8" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="8" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="21">
+      <c r="A26" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="8" t="s">
+      <c r="C26" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="8" t="s">
+      <c r="C27" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="26.25">
+      <c r="A29" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="8"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="C31" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="56.25">
       <c r="A32" s="8"/>
       <c r="B32" s="2"/>
       <c r="C32" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="37.5">
       <c r="A33" s="8"/>
       <c r="B33" s="2"/>
       <c r="C33" s="8"/>
@@ -1037,6 +1046,16 @@
       <c r="A35" s="8"/>
       <c r="B35" s="2"/>
       <c r="C35" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="8"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+      <c r="A37" s="8"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
long run looks good
</commit_message>
<xml_diff>
--- a/RiskParity_Holdings_Constraints.xlsx
+++ b/RiskParity_Holdings_Constraints.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="92">
   <si>
     <t>Asset</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Metals</t>
+  </si>
+  <si>
+    <t>FNZ</t>
   </si>
   <si>
     <t>Bonds</t>
@@ -751,7 +754,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>82</v>
@@ -779,7 +782,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -801,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -817,13 +820,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -853,7 +856,7 @@
         <v>73</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>56</v>
@@ -867,7 +870,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
@@ -878,7 +881,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
@@ -922,7 +925,7 @@
         <v>34</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
@@ -955,7 +958,7 @@
         <v>76</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">

</xml_diff>